<commit_message>
format group in order of session time
</commit_message>
<xml_diff>
--- a/Excel_template.xlsx
+++ b/Excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kenneth.McMillan\Dropbox\2.PYTHON_PROJECTS\SPORTS_DATABASES\Operations_timetable_python\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82A414F6-FAA0-4375-BBFE-929B06438C1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F781D908-B7D0-40D6-9D09-799A24012BC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="960" windowWidth="21840" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -744,6 +744,120 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -758,120 +872,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1318,8 +1318,8 @@
   </sheetPr>
   <dimension ref="A1:Q89"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A50" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38:XFD38"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A54" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="O35" sqref="O35:P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1357,72 +1357,72 @@
     </row>
     <row r="2" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="71" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
-      <c r="G2" s="34"/>
-      <c r="H2" s="34"/>
-      <c r="I2" s="34"/>
-      <c r="J2" s="34"/>
-      <c r="K2" s="34"/>
-      <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-      <c r="N2" s="34"/>
-      <c r="O2" s="67" t="str">
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="72"/>
+      <c r="N2" s="72"/>
+      <c r="O2" s="46" t="str">
         <f>"Week beginning" &amp; CHAR(10) &amp; TEXT(C4,"ddd-dd-mmm") &amp; " W-" &amp; WEEKNUM(C4)</f>
         <v>Week beginning
 Sat-00-Jan W-0</v>
       </c>
-      <c r="P2" s="68"/>
+      <c r="P2" s="47"/>
       <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:17" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="36"/>
-      <c r="D3" s="36"/>
-      <c r="E3" s="36"/>
-      <c r="F3" s="36"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="36"/>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="36"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="70"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="67"/>
+      <c r="D3" s="67"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="67"/>
+      <c r="H3" s="67"/>
+      <c r="I3" s="67"/>
+      <c r="J3" s="67"/>
+      <c r="K3" s="67"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="67"/>
+      <c r="N3" s="67"/>
+      <c r="O3" s="48"/>
+      <c r="P3" s="49"/>
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
-      <c r="B4" s="71" t="s">
+      <c r="B4" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="60"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="60"/>
-      <c r="I4" s="47"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="47"/>
-      <c r="L4" s="60"/>
-      <c r="M4" s="47"/>
-      <c r="N4" s="60"/>
-      <c r="O4" s="47"/>
-      <c r="P4" s="60"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="32"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="32"/>
+      <c r="P4" s="36"/>
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17" ht="25.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="3"/>
-      <c r="B5" s="72"/>
+      <c r="B5" s="31"/>
       <c r="C5" s="18" t="s">
         <v>32</v>
       </c>
@@ -1472,20 +1472,20 @@
       <c r="B6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="46"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="46"/>
-      <c r="F6" s="49"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="46"/>
-      <c r="J6" s="49"/>
-      <c r="K6" s="46"/>
-      <c r="L6" s="49"/>
-      <c r="M6" s="46"/>
-      <c r="N6" s="49"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="49"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="43"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="43"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="43"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="43"/>
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1493,19 +1493,19 @@
       <c r="B7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="42"/>
+      <c r="C7" s="35"/>
       <c r="D7" s="44"/>
-      <c r="E7" s="42"/>
+      <c r="E7" s="35"/>
       <c r="F7" s="44"/>
-      <c r="G7" s="42"/>
+      <c r="G7" s="35"/>
       <c r="H7" s="44"/>
-      <c r="I7" s="42"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="44"/>
-      <c r="K7" s="42"/>
+      <c r="K7" s="35"/>
       <c r="L7" s="44"/>
-      <c r="M7" s="42"/>
+      <c r="M7" s="35"/>
       <c r="N7" s="44"/>
-      <c r="O7" s="42"/>
+      <c r="O7" s="35"/>
       <c r="P7" s="44"/>
       <c r="Q7" s="3"/>
     </row>
@@ -1514,19 +1514,19 @@
       <c r="B8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="37"/>
+      <c r="C8" s="41"/>
       <c r="D8" s="39"/>
-      <c r="E8" s="37"/>
+      <c r="E8" s="41"/>
       <c r="F8" s="39"/>
-      <c r="G8" s="37"/>
+      <c r="G8" s="41"/>
       <c r="H8" s="39"/>
-      <c r="I8" s="37"/>
+      <c r="I8" s="41"/>
       <c r="J8" s="39"/>
-      <c r="K8" s="37"/>
+      <c r="K8" s="41"/>
       <c r="L8" s="39"/>
-      <c r="M8" s="37"/>
+      <c r="M8" s="41"/>
       <c r="N8" s="39"/>
-      <c r="O8" s="37"/>
+      <c r="O8" s="41"/>
       <c r="P8" s="39"/>
       <c r="Q8" s="3"/>
     </row>
@@ -1535,19 +1535,19 @@
       <c r="B9" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="38"/>
+      <c r="C9" s="42"/>
       <c r="D9" s="40"/>
-      <c r="E9" s="38"/>
+      <c r="E9" s="42"/>
       <c r="F9" s="40"/>
-      <c r="G9" s="38"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="40"/>
-      <c r="I9" s="38"/>
+      <c r="I9" s="42"/>
       <c r="J9" s="40"/>
-      <c r="K9" s="38"/>
+      <c r="K9" s="42"/>
       <c r="L9" s="40"/>
-      <c r="M9" s="38"/>
+      <c r="M9" s="42"/>
       <c r="N9" s="40"/>
-      <c r="O9" s="38"/>
+      <c r="O9" s="42"/>
       <c r="P9" s="40"/>
       <c r="Q9" s="3"/>
     </row>
@@ -1556,20 +1556,20 @@
       <c r="B10" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="43"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="43"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="43"/>
-      <c r="K10" s="41"/>
-      <c r="L10" s="43"/>
-      <c r="M10" s="41"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="41"/>
-      <c r="P10" s="43"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="45"/>
+      <c r="J10" s="50"/>
+      <c r="K10" s="45"/>
+      <c r="L10" s="50"/>
+      <c r="M10" s="45"/>
+      <c r="N10" s="50"/>
+      <c r="O10" s="45"/>
+      <c r="P10" s="50"/>
       <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1577,19 +1577,19 @@
       <c r="B11" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="42"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="44"/>
-      <c r="E11" s="42"/>
+      <c r="E11" s="35"/>
       <c r="F11" s="44"/>
-      <c r="G11" s="42"/>
+      <c r="G11" s="35"/>
       <c r="H11" s="44"/>
-      <c r="I11" s="42"/>
+      <c r="I11" s="35"/>
       <c r="J11" s="44"/>
-      <c r="K11" s="42"/>
+      <c r="K11" s="35"/>
       <c r="L11" s="44"/>
-      <c r="M11" s="42"/>
+      <c r="M11" s="35"/>
       <c r="N11" s="44"/>
-      <c r="O11" s="42"/>
+      <c r="O11" s="35"/>
       <c r="P11" s="44"/>
       <c r="Q11" s="3"/>
     </row>
@@ -1598,19 +1598,19 @@
       <c r="B12" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="37"/>
+      <c r="C12" s="41"/>
       <c r="D12" s="39"/>
-      <c r="E12" s="37"/>
+      <c r="E12" s="41"/>
       <c r="F12" s="39"/>
-      <c r="G12" s="37"/>
+      <c r="G12" s="41"/>
       <c r="H12" s="39"/>
-      <c r="I12" s="37"/>
+      <c r="I12" s="41"/>
       <c r="J12" s="39"/>
-      <c r="K12" s="37"/>
+      <c r="K12" s="41"/>
       <c r="L12" s="39"/>
-      <c r="M12" s="37"/>
+      <c r="M12" s="41"/>
       <c r="N12" s="39"/>
-      <c r="O12" s="37"/>
+      <c r="O12" s="41"/>
       <c r="P12" s="39"/>
       <c r="Q12" s="3"/>
     </row>
@@ -1619,19 +1619,19 @@
       <c r="B13" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="38"/>
+      <c r="C13" s="42"/>
       <c r="D13" s="40"/>
-      <c r="E13" s="38"/>
+      <c r="E13" s="42"/>
       <c r="F13" s="40"/>
-      <c r="G13" s="38"/>
+      <c r="G13" s="42"/>
       <c r="H13" s="40"/>
-      <c r="I13" s="38"/>
+      <c r="I13" s="42"/>
       <c r="J13" s="40"/>
-      <c r="K13" s="38"/>
+      <c r="K13" s="42"/>
       <c r="L13" s="40"/>
-      <c r="M13" s="38"/>
+      <c r="M13" s="42"/>
       <c r="N13" s="40"/>
-      <c r="O13" s="38"/>
+      <c r="O13" s="42"/>
       <c r="P13" s="40"/>
       <c r="Q13" s="3"/>
     </row>
@@ -1640,20 +1640,20 @@
       <c r="B14" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="41"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="43"/>
-      <c r="G14" s="41"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="41"/>
-      <c r="J14" s="43"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="43"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="43"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="43"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="50"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="50"/>
+      <c r="G14" s="45"/>
+      <c r="H14" s="50"/>
+      <c r="I14" s="45"/>
+      <c r="J14" s="50"/>
+      <c r="K14" s="45"/>
+      <c r="L14" s="50"/>
+      <c r="M14" s="45"/>
+      <c r="N14" s="50"/>
+      <c r="O14" s="45"/>
+      <c r="P14" s="50"/>
       <c r="Q14" s="3"/>
     </row>
     <row r="15" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1661,19 +1661,19 @@
       <c r="B15" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C15" s="42"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="44"/>
-      <c r="E15" s="42"/>
+      <c r="E15" s="35"/>
       <c r="F15" s="44"/>
-      <c r="G15" s="42"/>
+      <c r="G15" s="35"/>
       <c r="H15" s="44"/>
-      <c r="I15" s="42"/>
+      <c r="I15" s="35"/>
       <c r="J15" s="44"/>
-      <c r="K15" s="42"/>
+      <c r="K15" s="35"/>
       <c r="L15" s="44"/>
-      <c r="M15" s="42"/>
+      <c r="M15" s="35"/>
       <c r="N15" s="44"/>
-      <c r="O15" s="42"/>
+      <c r="O15" s="35"/>
       <c r="P15" s="44"/>
       <c r="Q15" s="3"/>
     </row>
@@ -1682,19 +1682,19 @@
       <c r="B16" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="37"/>
+      <c r="C16" s="41"/>
       <c r="D16" s="39"/>
-      <c r="E16" s="37"/>
+      <c r="E16" s="41"/>
       <c r="F16" s="39"/>
-      <c r="G16" s="37"/>
+      <c r="G16" s="41"/>
       <c r="H16" s="39"/>
-      <c r="I16" s="37"/>
+      <c r="I16" s="41"/>
       <c r="J16" s="39"/>
-      <c r="K16" s="37"/>
+      <c r="K16" s="41"/>
       <c r="L16" s="39"/>
-      <c r="M16" s="37"/>
+      <c r="M16" s="41"/>
       <c r="N16" s="39"/>
-      <c r="O16" s="37"/>
+      <c r="O16" s="41"/>
       <c r="P16" s="39"/>
       <c r="Q16" s="3"/>
     </row>
@@ -1703,19 +1703,19 @@
       <c r="B17" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C17" s="38"/>
+      <c r="C17" s="42"/>
       <c r="D17" s="40"/>
-      <c r="E17" s="38"/>
+      <c r="E17" s="42"/>
       <c r="F17" s="40"/>
-      <c r="G17" s="38"/>
+      <c r="G17" s="42"/>
       <c r="H17" s="40"/>
-      <c r="I17" s="38"/>
+      <c r="I17" s="42"/>
       <c r="J17" s="40"/>
-      <c r="K17" s="38"/>
+      <c r="K17" s="42"/>
       <c r="L17" s="40"/>
-      <c r="M17" s="38"/>
+      <c r="M17" s="42"/>
       <c r="N17" s="40"/>
-      <c r="O17" s="38"/>
+      <c r="O17" s="42"/>
       <c r="P17" s="40"/>
       <c r="Q17" s="3"/>
     </row>
@@ -1724,20 +1724,20 @@
       <c r="B18" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="41"/>
-      <c r="D18" s="43"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="41"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="41"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="41"/>
-      <c r="L18" s="43"/>
-      <c r="M18" s="41"/>
-      <c r="N18" s="43"/>
-      <c r="O18" s="41"/>
-      <c r="P18" s="43"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="50"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="50"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="50"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="45"/>
+      <c r="L18" s="50"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="50"/>
+      <c r="O18" s="45"/>
+      <c r="P18" s="50"/>
       <c r="Q18" s="3"/>
     </row>
     <row r="19" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1745,19 +1745,19 @@
       <c r="B19" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="42"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="44"/>
-      <c r="E19" s="42"/>
+      <c r="E19" s="35"/>
       <c r="F19" s="44"/>
-      <c r="G19" s="42"/>
+      <c r="G19" s="35"/>
       <c r="H19" s="44"/>
-      <c r="I19" s="42"/>
+      <c r="I19" s="35"/>
       <c r="J19" s="44"/>
-      <c r="K19" s="42"/>
+      <c r="K19" s="35"/>
       <c r="L19" s="44"/>
-      <c r="M19" s="42"/>
+      <c r="M19" s="35"/>
       <c r="N19" s="44"/>
-      <c r="O19" s="42"/>
+      <c r="O19" s="35"/>
       <c r="P19" s="44"/>
       <c r="Q19" s="3"/>
     </row>
@@ -1766,19 +1766,19 @@
       <c r="B20" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="37"/>
+      <c r="C20" s="41"/>
       <c r="D20" s="39"/>
-      <c r="E20" s="37"/>
+      <c r="E20" s="41"/>
       <c r="F20" s="39"/>
-      <c r="G20" s="37"/>
+      <c r="G20" s="41"/>
       <c r="H20" s="39"/>
-      <c r="I20" s="37"/>
+      <c r="I20" s="41"/>
       <c r="J20" s="39"/>
-      <c r="K20" s="37"/>
+      <c r="K20" s="41"/>
       <c r="L20" s="39"/>
-      <c r="M20" s="37"/>
+      <c r="M20" s="41"/>
       <c r="N20" s="39"/>
-      <c r="O20" s="37"/>
+      <c r="O20" s="41"/>
       <c r="P20" s="39"/>
       <c r="Q20" s="3"/>
     </row>
@@ -1787,19 +1787,19 @@
       <c r="B21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="38"/>
+      <c r="C21" s="42"/>
       <c r="D21" s="40"/>
-      <c r="E21" s="38"/>
+      <c r="E21" s="42"/>
       <c r="F21" s="40"/>
-      <c r="G21" s="38"/>
+      <c r="G21" s="42"/>
       <c r="H21" s="40"/>
-      <c r="I21" s="38"/>
+      <c r="I21" s="42"/>
       <c r="J21" s="40"/>
-      <c r="K21" s="38"/>
+      <c r="K21" s="42"/>
       <c r="L21" s="40"/>
-      <c r="M21" s="38"/>
+      <c r="M21" s="42"/>
       <c r="N21" s="40"/>
-      <c r="O21" s="38"/>
+      <c r="O21" s="42"/>
       <c r="P21" s="40"/>
       <c r="Q21" s="3"/>
     </row>
@@ -1808,20 +1808,20 @@
       <c r="B22" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="41"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="41"/>
-      <c r="L22" s="43"/>
-      <c r="M22" s="41"/>
-      <c r="N22" s="43"/>
-      <c r="O22" s="41"/>
-      <c r="P22" s="43"/>
+      <c r="C22" s="45"/>
+      <c r="D22" s="50"/>
+      <c r="E22" s="45"/>
+      <c r="F22" s="50"/>
+      <c r="G22" s="45"/>
+      <c r="H22" s="50"/>
+      <c r="I22" s="45"/>
+      <c r="J22" s="50"/>
+      <c r="K22" s="45"/>
+      <c r="L22" s="50"/>
+      <c r="M22" s="45"/>
+      <c r="N22" s="50"/>
+      <c r="O22" s="45"/>
+      <c r="P22" s="50"/>
       <c r="Q22" s="3"/>
     </row>
     <row r="23" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1829,19 +1829,19 @@
       <c r="B23" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="C23" s="42"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="44"/>
-      <c r="E23" s="42"/>
+      <c r="E23" s="35"/>
       <c r="F23" s="44"/>
-      <c r="G23" s="42"/>
+      <c r="G23" s="35"/>
       <c r="H23" s="44"/>
-      <c r="I23" s="42"/>
+      <c r="I23" s="35"/>
       <c r="J23" s="44"/>
-      <c r="K23" s="42"/>
+      <c r="K23" s="35"/>
       <c r="L23" s="44"/>
-      <c r="M23" s="42"/>
+      <c r="M23" s="35"/>
       <c r="N23" s="44"/>
-      <c r="O23" s="42"/>
+      <c r="O23" s="35"/>
       <c r="P23" s="44"/>
       <c r="Q23" s="3"/>
     </row>
@@ -1850,19 +1850,19 @@
       <c r="B24" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="37"/>
+      <c r="C24" s="41"/>
       <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
+      <c r="E24" s="41"/>
       <c r="F24" s="39"/>
-      <c r="G24" s="37"/>
+      <c r="G24" s="41"/>
       <c r="H24" s="39"/>
-      <c r="I24" s="37"/>
+      <c r="I24" s="41"/>
       <c r="J24" s="39"/>
-      <c r="K24" s="37"/>
+      <c r="K24" s="41"/>
       <c r="L24" s="39"/>
-      <c r="M24" s="37"/>
+      <c r="M24" s="41"/>
       <c r="N24" s="39"/>
-      <c r="O24" s="37"/>
+      <c r="O24" s="41"/>
       <c r="P24" s="39"/>
       <c r="Q24" s="3"/>
     </row>
@@ -1871,19 +1871,19 @@
       <c r="B25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="38"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="40"/>
-      <c r="E25" s="38"/>
+      <c r="E25" s="42"/>
       <c r="F25" s="40"/>
-      <c r="G25" s="38"/>
+      <c r="G25" s="42"/>
       <c r="H25" s="40"/>
-      <c r="I25" s="38"/>
+      <c r="I25" s="42"/>
       <c r="J25" s="40"/>
-      <c r="K25" s="38"/>
+      <c r="K25" s="42"/>
       <c r="L25" s="40"/>
-      <c r="M25" s="38"/>
+      <c r="M25" s="42"/>
       <c r="N25" s="40"/>
-      <c r="O25" s="38"/>
+      <c r="O25" s="42"/>
       <c r="P25" s="40"/>
       <c r="Q25" s="3"/>
     </row>
@@ -1892,20 +1892,20 @@
       <c r="B26" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="43"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="41"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="41"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="43"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="43"/>
-      <c r="O26" s="41"/>
-      <c r="P26" s="43"/>
+      <c r="C26" s="45"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="45"/>
+      <c r="F26" s="50"/>
+      <c r="G26" s="45"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="45"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="50"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="50"/>
+      <c r="O26" s="45"/>
+      <c r="P26" s="50"/>
       <c r="Q26" s="3"/>
     </row>
     <row r="27" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -1913,58 +1913,58 @@
       <c r="B27" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="42"/>
+      <c r="C27" s="35"/>
       <c r="D27" s="44"/>
-      <c r="E27" s="42"/>
+      <c r="E27" s="35"/>
       <c r="F27" s="44"/>
-      <c r="G27" s="42"/>
+      <c r="G27" s="35"/>
       <c r="H27" s="44"/>
-      <c r="I27" s="42"/>
+      <c r="I27" s="35"/>
       <c r="J27" s="44"/>
-      <c r="K27" s="42"/>
+      <c r="K27" s="35"/>
       <c r="L27" s="44"/>
-      <c r="M27" s="42"/>
+      <c r="M27" s="35"/>
       <c r="N27" s="44"/>
-      <c r="O27" s="42"/>
+      <c r="O27" s="35"/>
       <c r="P27" s="44"/>
       <c r="Q27" s="3"/>
     </row>
     <row r="28" spans="1:17" ht="32.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="12"/>
-      <c r="C28" s="37"/>
+      <c r="C28" s="41"/>
       <c r="D28" s="39"/>
-      <c r="E28" s="37"/>
+      <c r="E28" s="41"/>
       <c r="F28" s="39"/>
-      <c r="G28" s="37"/>
+      <c r="G28" s="41"/>
       <c r="H28" s="39"/>
-      <c r="I28" s="37"/>
+      <c r="I28" s="41"/>
       <c r="J28" s="39"/>
-      <c r="K28" s="37"/>
+      <c r="K28" s="41"/>
       <c r="L28" s="39"/>
-      <c r="M28" s="37"/>
+      <c r="M28" s="41"/>
       <c r="N28" s="39"/>
-      <c r="O28" s="37"/>
+      <c r="O28" s="41"/>
       <c r="P28" s="39"/>
       <c r="Q28" s="3"/>
     </row>
     <row r="29" spans="1:17" ht="32.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A29" s="3"/>
       <c r="B29" s="13"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="57"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="57"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="57"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="57"/>
-      <c r="M29" s="45"/>
-      <c r="N29" s="57"/>
-      <c r="O29" s="45"/>
-      <c r="P29" s="57"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="56"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="56"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="56"/>
+      <c r="K29" s="55"/>
+      <c r="L29" s="56"/>
+      <c r="M29" s="55"/>
+      <c r="N29" s="56"/>
+      <c r="O29" s="55"/>
+      <c r="P29" s="56"/>
       <c r="Q29" s="3"/>
     </row>
     <row r="30" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -2024,93 +2024,72 @@
     </row>
     <row r="33" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="59"/>
-      <c r="E33" s="59"/>
-      <c r="F33" s="59"/>
-      <c r="G33" s="59"/>
-      <c r="H33" s="59"/>
-      <c r="I33" s="59"/>
-      <c r="J33" s="59"/>
-      <c r="K33" s="59"/>
-      <c r="L33" s="59"/>
-      <c r="M33" s="59"/>
-      <c r="N33" s="59"/>
-      <c r="O33" s="67" t="str">
+      <c r="C33" s="65"/>
+      <c r="D33" s="65"/>
+      <c r="E33" s="65"/>
+      <c r="F33" s="65"/>
+      <c r="G33" s="65"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
+      <c r="K33" s="65"/>
+      <c r="L33" s="65"/>
+      <c r="M33" s="65"/>
+      <c r="N33" s="65"/>
+      <c r="O33" s="46" t="str">
         <f>O2</f>
         <v>Week beginning
 Sat-00-Jan W-0</v>
       </c>
-      <c r="P33" s="68"/>
+      <c r="P33" s="47"/>
       <c r="Q33" s="3"/>
     </row>
     <row r="34" spans="1:17" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3"/>
-      <c r="B34" s="35"/>
-      <c r="C34" s="36"/>
-      <c r="D34" s="36"/>
-      <c r="E34" s="36"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="36"/>
-      <c r="H34" s="36"/>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
-      <c r="K34" s="36"/>
-      <c r="L34" s="36"/>
-      <c r="M34" s="36"/>
-      <c r="N34" s="36"/>
-      <c r="O34" s="69"/>
-      <c r="P34" s="70"/>
+      <c r="B34" s="66"/>
+      <c r="C34" s="67"/>
+      <c r="D34" s="67"/>
+      <c r="E34" s="67"/>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="I34" s="67"/>
+      <c r="J34" s="67"/>
+      <c r="K34" s="67"/>
+      <c r="L34" s="67"/>
+      <c r="M34" s="67"/>
+      <c r="N34" s="67"/>
+      <c r="O34" s="48"/>
+      <c r="P34" s="49"/>
       <c r="Q34" s="3"/>
     </row>
     <row r="35" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
-      <c r="B35" s="65" t="s">
+      <c r="B35" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C35" s="47">
-        <f>C4</f>
-        <v>0</v>
-      </c>
-      <c r="D35" s="48"/>
-      <c r="E35" s="47">
-        <f t="shared" ref="E35" si="0">E4</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="48"/>
-      <c r="G35" s="47">
-        <f t="shared" ref="G35" si="1">G4</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="48"/>
-      <c r="I35" s="47">
-        <f t="shared" ref="I35" si="2">I4</f>
-        <v>0</v>
-      </c>
-      <c r="J35" s="48"/>
-      <c r="K35" s="47">
-        <f t="shared" ref="K35:M35" si="3">K4</f>
-        <v>0</v>
-      </c>
-      <c r="L35" s="48"/>
-      <c r="M35" s="47">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="N35" s="48"/>
-      <c r="O35" s="47">
-        <f t="shared" ref="O35" si="4">O4</f>
-        <v>0</v>
-      </c>
-      <c r="P35" s="48"/>
+      <c r="C35" s="32"/>
+      <c r="D35" s="33"/>
+      <c r="E35" s="32"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="32"/>
+      <c r="H35" s="33"/>
+      <c r="I35" s="32"/>
+      <c r="J35" s="33"/>
+      <c r="K35" s="32"/>
+      <c r="L35" s="33"/>
+      <c r="M35" s="32"/>
+      <c r="N35" s="33"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="33"/>
       <c r="Q35" s="3"/>
     </row>
     <row r="36" spans="1:17" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3"/>
-      <c r="B36" s="66"/>
+      <c r="B36" s="38"/>
       <c r="C36" s="18" t="s">
         <v>32</v>
       </c>
@@ -2160,20 +2139,20 @@
       <c r="B37" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C37" s="46"/>
-      <c r="D37" s="49"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="49"/>
+      <c r="C37" s="34"/>
+      <c r="D37" s="43"/>
+      <c r="E37" s="34"/>
+      <c r="F37" s="43"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="34"/>
+      <c r="J37" s="43"/>
+      <c r="K37" s="34"/>
+      <c r="L37" s="43"/>
+      <c r="M37" s="34"/>
+      <c r="N37" s="43"/>
+      <c r="O37" s="34"/>
+      <c r="P37" s="43"/>
       <c r="Q37" s="3"/>
     </row>
     <row r="38" spans="1:17" ht="37.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2181,40 +2160,40 @@
       <c r="B38" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C38" s="42"/>
+      <c r="C38" s="35"/>
       <c r="D38" s="44"/>
-      <c r="E38" s="42"/>
+      <c r="E38" s="35"/>
       <c r="F38" s="44"/>
-      <c r="G38" s="42"/>
+      <c r="G38" s="35"/>
       <c r="H38" s="44"/>
-      <c r="I38" s="42"/>
+      <c r="I38" s="35"/>
       <c r="J38" s="44"/>
-      <c r="K38" s="42"/>
+      <c r="K38" s="35"/>
       <c r="L38" s="44"/>
-      <c r="M38" s="42"/>
+      <c r="M38" s="35"/>
       <c r="N38" s="44"/>
-      <c r="O38" s="42"/>
+      <c r="O38" s="35"/>
       <c r="P38" s="44"/>
       <c r="Q38" s="3"/>
     </row>
-    <row r="39" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:17" ht="21" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C39" s="37"/>
+      <c r="C39" s="41"/>
       <c r="D39" s="39"/>
-      <c r="E39" s="37"/>
+      <c r="E39" s="41"/>
       <c r="F39" s="39"/>
-      <c r="G39" s="37"/>
+      <c r="G39" s="41"/>
       <c r="H39" s="39"/>
-      <c r="I39" s="37"/>
+      <c r="I39" s="41"/>
       <c r="J39" s="39"/>
-      <c r="K39" s="37"/>
+      <c r="K39" s="41"/>
       <c r="L39" s="39"/>
-      <c r="M39" s="37"/>
+      <c r="M39" s="41"/>
       <c r="N39" s="39"/>
-      <c r="O39" s="37"/>
+      <c r="O39" s="41"/>
       <c r="P39" s="39"/>
       <c r="Q39" s="3"/>
     </row>
@@ -2223,41 +2202,41 @@
       <c r="B40" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C40" s="38"/>
+      <c r="C40" s="42"/>
       <c r="D40" s="40"/>
-      <c r="E40" s="38"/>
+      <c r="E40" s="42"/>
       <c r="F40" s="40"/>
-      <c r="G40" s="38"/>
+      <c r="G40" s="42"/>
       <c r="H40" s="40"/>
-      <c r="I40" s="38"/>
+      <c r="I40" s="42"/>
       <c r="J40" s="40"/>
-      <c r="K40" s="38"/>
+      <c r="K40" s="42"/>
       <c r="L40" s="40"/>
-      <c r="M40" s="38"/>
+      <c r="M40" s="42"/>
       <c r="N40" s="40"/>
-      <c r="O40" s="38"/>
+      <c r="O40" s="42"/>
       <c r="P40" s="40"/>
       <c r="Q40" s="3"/>
     </row>
-    <row r="41" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="43"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="43"/>
-      <c r="G41" s="41"/>
-      <c r="H41" s="43"/>
-      <c r="I41" s="41"/>
-      <c r="J41" s="43"/>
-      <c r="K41" s="41"/>
-      <c r="L41" s="43"/>
-      <c r="M41" s="41"/>
-      <c r="N41" s="43"/>
-      <c r="O41" s="41"/>
-      <c r="P41" s="43"/>
+      <c r="C41" s="45"/>
+      <c r="D41" s="50"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="45"/>
+      <c r="H41" s="50"/>
+      <c r="I41" s="45"/>
+      <c r="J41" s="50"/>
+      <c r="K41" s="45"/>
+      <c r="L41" s="50"/>
+      <c r="M41" s="45"/>
+      <c r="N41" s="50"/>
+      <c r="O41" s="45"/>
+      <c r="P41" s="50"/>
       <c r="Q41" s="3"/>
     </row>
     <row r="42" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2265,40 +2244,40 @@
       <c r="B42" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C42" s="42"/>
+      <c r="C42" s="35"/>
       <c r="D42" s="44"/>
-      <c r="E42" s="42"/>
+      <c r="E42" s="35"/>
       <c r="F42" s="44"/>
-      <c r="G42" s="42"/>
+      <c r="G42" s="35"/>
       <c r="H42" s="44"/>
-      <c r="I42" s="42"/>
+      <c r="I42" s="35"/>
       <c r="J42" s="44"/>
-      <c r="K42" s="42"/>
+      <c r="K42" s="35"/>
       <c r="L42" s="44"/>
-      <c r="M42" s="42"/>
+      <c r="M42" s="35"/>
       <c r="N42" s="44"/>
-      <c r="O42" s="42"/>
+      <c r="O42" s="35"/>
       <c r="P42" s="44"/>
       <c r="Q42" s="3"/>
     </row>
-    <row r="43" spans="1:17" ht="32.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C43" s="37"/>
+      <c r="C43" s="41"/>
       <c r="D43" s="39"/>
-      <c r="E43" s="37"/>
+      <c r="E43" s="41"/>
       <c r="F43" s="39"/>
-      <c r="G43" s="37"/>
+      <c r="G43" s="41"/>
       <c r="H43" s="39"/>
-      <c r="I43" s="37"/>
+      <c r="I43" s="41"/>
       <c r="J43" s="39"/>
-      <c r="K43" s="37"/>
+      <c r="K43" s="41"/>
       <c r="L43" s="39"/>
-      <c r="M43" s="37"/>
+      <c r="M43" s="41"/>
       <c r="N43" s="39"/>
-      <c r="O43" s="37"/>
+      <c r="O43" s="41"/>
       <c r="P43" s="39"/>
       <c r="Q43" s="3"/>
     </row>
@@ -2307,19 +2286,19 @@
       <c r="B44" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C44" s="38"/>
+      <c r="C44" s="42"/>
       <c r="D44" s="40"/>
-      <c r="E44" s="38"/>
+      <c r="E44" s="42"/>
       <c r="F44" s="40"/>
-      <c r="G44" s="38"/>
+      <c r="G44" s="42"/>
       <c r="H44" s="40"/>
-      <c r="I44" s="38"/>
+      <c r="I44" s="42"/>
       <c r="J44" s="40"/>
-      <c r="K44" s="38"/>
+      <c r="K44" s="42"/>
       <c r="L44" s="40"/>
-      <c r="M44" s="38"/>
+      <c r="M44" s="42"/>
       <c r="N44" s="40"/>
-      <c r="O44" s="38"/>
+      <c r="O44" s="42"/>
       <c r="P44" s="40"/>
       <c r="Q44" s="3"/>
     </row>
@@ -2328,20 +2307,20 @@
       <c r="B45" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="43"/>
-      <c r="E45" s="41"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="41"/>
-      <c r="H45" s="43"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="43"/>
-      <c r="K45" s="41"/>
-      <c r="L45" s="43"/>
-      <c r="M45" s="41"/>
-      <c r="N45" s="43"/>
-      <c r="O45" s="41"/>
-      <c r="P45" s="43"/>
+      <c r="C45" s="45"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="50"/>
+      <c r="G45" s="45"/>
+      <c r="H45" s="50"/>
+      <c r="I45" s="45"/>
+      <c r="J45" s="50"/>
+      <c r="K45" s="45"/>
+      <c r="L45" s="50"/>
+      <c r="M45" s="45"/>
+      <c r="N45" s="50"/>
+      <c r="O45" s="45"/>
+      <c r="P45" s="50"/>
       <c r="Q45" s="3"/>
     </row>
     <row r="46" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2349,19 +2328,19 @@
       <c r="B46" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="42"/>
+      <c r="C46" s="35"/>
       <c r="D46" s="44"/>
-      <c r="E46" s="42"/>
+      <c r="E46" s="35"/>
       <c r="F46" s="44"/>
-      <c r="G46" s="42"/>
+      <c r="G46" s="35"/>
       <c r="H46" s="44"/>
-      <c r="I46" s="42"/>
+      <c r="I46" s="35"/>
       <c r="J46" s="44"/>
-      <c r="K46" s="42"/>
+      <c r="K46" s="35"/>
       <c r="L46" s="44"/>
-      <c r="M46" s="42"/>
+      <c r="M46" s="35"/>
       <c r="N46" s="44"/>
-      <c r="O46" s="42"/>
+      <c r="O46" s="35"/>
       <c r="P46" s="44"/>
       <c r="Q46" s="3"/>
     </row>
@@ -2370,20 +2349,20 @@
       <c r="B47" s="22" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="30"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="31"/>
-      <c r="G47" s="31"/>
-      <c r="H47" s="31"/>
-      <c r="I47" s="31"/>
-      <c r="J47" s="31"/>
-      <c r="K47" s="31"/>
-      <c r="L47" s="31"/>
-      <c r="M47" s="31"/>
-      <c r="N47" s="31"/>
-      <c r="O47" s="31"/>
-      <c r="P47" s="32"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="69"/>
+      <c r="M47" s="69"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="69"/>
+      <c r="P47" s="70"/>
       <c r="Q47" s="3"/>
     </row>
     <row r="48" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2454,20 +2433,20 @@
       <c r="B51" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="C51" s="41"/>
-      <c r="D51" s="43"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="41"/>
-      <c r="H51" s="43"/>
-      <c r="I51" s="41"/>
-      <c r="J51" s="43"/>
-      <c r="K51" s="41"/>
-      <c r="L51" s="43"/>
-      <c r="M51" s="41"/>
-      <c r="N51" s="43"/>
-      <c r="O51" s="41"/>
-      <c r="P51" s="43"/>
+      <c r="C51" s="45"/>
+      <c r="D51" s="50"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="50"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="45"/>
+      <c r="J51" s="50"/>
+      <c r="K51" s="45"/>
+      <c r="L51" s="50"/>
+      <c r="M51" s="45"/>
+      <c r="N51" s="50"/>
+      <c r="O51" s="45"/>
+      <c r="P51" s="50"/>
       <c r="Q51" s="3"/>
     </row>
     <row r="52" spans="1:17" ht="27" customHeight="1" x14ac:dyDescent="0.35">
@@ -2475,19 +2454,19 @@
       <c r="B52" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C52" s="42"/>
+      <c r="C52" s="35"/>
       <c r="D52" s="44"/>
-      <c r="E52" s="42"/>
+      <c r="E52" s="35"/>
       <c r="F52" s="44"/>
-      <c r="G52" s="42"/>
+      <c r="G52" s="35"/>
       <c r="H52" s="44"/>
-      <c r="I52" s="42"/>
+      <c r="I52" s="35"/>
       <c r="J52" s="44"/>
-      <c r="K52" s="42"/>
+      <c r="K52" s="35"/>
       <c r="L52" s="44"/>
-      <c r="M52" s="42"/>
+      <c r="M52" s="35"/>
       <c r="N52" s="44"/>
-      <c r="O52" s="42"/>
+      <c r="O52" s="35"/>
       <c r="P52" s="44"/>
       <c r="Q52" s="3"/>
     </row>
@@ -2496,38 +2475,38 @@
       <c r="B53" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="37"/>
+      <c r="C53" s="41"/>
       <c r="D53" s="39"/>
-      <c r="E53" s="37"/>
+      <c r="E53" s="41"/>
       <c r="F53" s="39"/>
-      <c r="G53" s="37"/>
+      <c r="G53" s="41"/>
       <c r="H53" s="39"/>
-      <c r="I53" s="37"/>
+      <c r="I53" s="41"/>
       <c r="J53" s="39"/>
-      <c r="K53" s="37"/>
+      <c r="K53" s="41"/>
       <c r="L53" s="39"/>
-      <c r="M53" s="37"/>
+      <c r="M53" s="41"/>
       <c r="N53" s="39"/>
-      <c r="O53" s="37"/>
+      <c r="O53" s="41"/>
       <c r="P53" s="39"/>
       <c r="Q53" s="3"/>
     </row>
     <row r="54" spans="1:17" ht="23" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3"/>
       <c r="B54" s="13"/>
-      <c r="C54" s="38"/>
+      <c r="C54" s="42"/>
       <c r="D54" s="40"/>
-      <c r="E54" s="38"/>
+      <c r="E54" s="42"/>
       <c r="F54" s="40"/>
-      <c r="G54" s="38"/>
+      <c r="G54" s="42"/>
       <c r="H54" s="40"/>
-      <c r="I54" s="38"/>
+      <c r="I54" s="42"/>
       <c r="J54" s="40"/>
-      <c r="K54" s="38"/>
+      <c r="K54" s="42"/>
       <c r="L54" s="40"/>
-      <c r="M54" s="38"/>
+      <c r="M54" s="42"/>
       <c r="N54" s="40"/>
-      <c r="O54" s="38"/>
+      <c r="O54" s="42"/>
       <c r="P54" s="40"/>
       <c r="Q54" s="3"/>
     </row>
@@ -2536,38 +2515,38 @@
       <c r="B55" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="C55" s="41"/>
-      <c r="D55" s="43"/>
-      <c r="E55" s="41"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="41"/>
-      <c r="H55" s="43"/>
-      <c r="I55" s="41"/>
-      <c r="J55" s="43"/>
-      <c r="K55" s="41"/>
-      <c r="L55" s="43"/>
-      <c r="M55" s="41"/>
-      <c r="N55" s="43"/>
-      <c r="O55" s="41"/>
-      <c r="P55" s="43"/>
+      <c r="C55" s="45"/>
+      <c r="D55" s="50"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="50"/>
+      <c r="G55" s="45"/>
+      <c r="H55" s="50"/>
+      <c r="I55" s="45"/>
+      <c r="J55" s="50"/>
+      <c r="K55" s="45"/>
+      <c r="L55" s="50"/>
+      <c r="M55" s="45"/>
+      <c r="N55" s="50"/>
+      <c r="O55" s="45"/>
+      <c r="P55" s="50"/>
       <c r="Q55" s="3"/>
     </row>
     <row r="56" spans="1:17" ht="26.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="11"/>
-      <c r="C56" s="42"/>
+      <c r="C56" s="35"/>
       <c r="D56" s="44"/>
-      <c r="E56" s="42"/>
+      <c r="E56" s="35"/>
       <c r="F56" s="44"/>
-      <c r="G56" s="42"/>
+      <c r="G56" s="35"/>
       <c r="H56" s="44"/>
-      <c r="I56" s="42"/>
+      <c r="I56" s="35"/>
       <c r="J56" s="44"/>
-      <c r="K56" s="42"/>
+      <c r="K56" s="35"/>
       <c r="L56" s="44"/>
-      <c r="M56" s="42"/>
+      <c r="M56" s="35"/>
       <c r="N56" s="44"/>
-      <c r="O56" s="42"/>
+      <c r="O56" s="35"/>
       <c r="P56" s="44"/>
       <c r="Q56" s="3"/>
     </row>
@@ -2576,23 +2555,23 @@
       <c r="B57" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="C57" s="54"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="55"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="55"/>
-      <c r="N57" s="55"/>
-      <c r="O57" s="55"/>
-      <c r="P57" s="56"/>
+      <c r="C57" s="61"/>
+      <c r="D57" s="62"/>
+      <c r="E57" s="62"/>
+      <c r="F57" s="62"/>
+      <c r="G57" s="62"/>
+      <c r="H57" s="62"/>
+      <c r="I57" s="62"/>
+      <c r="J57" s="62"/>
+      <c r="K57" s="62"/>
+      <c r="L57" s="62"/>
+      <c r="M57" s="62"/>
+      <c r="N57" s="62"/>
+      <c r="O57" s="62"/>
+      <c r="P57" s="63"/>
       <c r="Q57" s="3"/>
     </row>
-    <row r="58" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:17" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3"/>
       <c r="B58" s="23" t="s">
         <v>45</v>
@@ -2613,7 +2592,7 @@
       <c r="P58" s="27"/>
       <c r="Q58" s="3"/>
     </row>
-    <row r="59" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:17" ht="55" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3"/>
       <c r="B59" s="23" t="s">
         <v>46</v>
@@ -2634,7 +2613,7 @@
       <c r="P59" s="27"/>
       <c r="Q59" s="3"/>
     </row>
-    <row r="60" spans="1:17" ht="53" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:17" ht="54" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3"/>
       <c r="B60" s="23" t="s">
         <v>47</v>
@@ -2655,7 +2634,7 @@
       <c r="P60" s="27"/>
       <c r="Q60" s="3"/>
     </row>
-    <row r="61" spans="1:17" ht="53.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:17" ht="54.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3"/>
       <c r="B61" s="23" t="s">
         <v>48</v>
@@ -2733,93 +2712,72 @@
     </row>
     <row r="65" spans="1:17" ht="26.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3"/>
-      <c r="B65" s="50" t="s">
+      <c r="B65" s="57" t="s">
         <v>39</v>
       </c>
-      <c r="C65" s="51"/>
-      <c r="D65" s="51"/>
-      <c r="E65" s="51"/>
-      <c r="F65" s="51"/>
-      <c r="G65" s="51"/>
-      <c r="H65" s="51"/>
-      <c r="I65" s="51"/>
-      <c r="J65" s="51"/>
-      <c r="K65" s="51"/>
-      <c r="L65" s="51"/>
-      <c r="M65" s="51"/>
-      <c r="N65" s="51"/>
-      <c r="O65" s="61" t="str">
+      <c r="C65" s="58"/>
+      <c r="D65" s="58"/>
+      <c r="E65" s="58"/>
+      <c r="F65" s="58"/>
+      <c r="G65" s="58"/>
+      <c r="H65" s="58"/>
+      <c r="I65" s="58"/>
+      <c r="J65" s="58"/>
+      <c r="K65" s="58"/>
+      <c r="L65" s="58"/>
+      <c r="M65" s="58"/>
+      <c r="N65" s="58"/>
+      <c r="O65" s="51" t="str">
         <f>O2</f>
         <v>Week beginning
 Sat-00-Jan W-0</v>
       </c>
-      <c r="P65" s="62"/>
+      <c r="P65" s="52"/>
       <c r="Q65" s="3"/>
     </row>
     <row r="66" spans="1:17" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3"/>
-      <c r="B66" s="52"/>
-      <c r="C66" s="53"/>
-      <c r="D66" s="53"/>
-      <c r="E66" s="53"/>
-      <c r="F66" s="53"/>
-      <c r="G66" s="53"/>
-      <c r="H66" s="53"/>
-      <c r="I66" s="53"/>
-      <c r="J66" s="53"/>
-      <c r="K66" s="53"/>
-      <c r="L66" s="53"/>
-      <c r="M66" s="53"/>
-      <c r="N66" s="53"/>
-      <c r="O66" s="63"/>
-      <c r="P66" s="64"/>
+      <c r="B66" s="59"/>
+      <c r="C66" s="60"/>
+      <c r="D66" s="60"/>
+      <c r="E66" s="60"/>
+      <c r="F66" s="60"/>
+      <c r="G66" s="60"/>
+      <c r="H66" s="60"/>
+      <c r="I66" s="60"/>
+      <c r="J66" s="60"/>
+      <c r="K66" s="60"/>
+      <c r="L66" s="60"/>
+      <c r="M66" s="60"/>
+      <c r="N66" s="60"/>
+      <c r="O66" s="53"/>
+      <c r="P66" s="54"/>
       <c r="Q66" s="3"/>
     </row>
     <row r="67" spans="1:17" ht="24.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3"/>
-      <c r="B67" s="65" t="s">
+      <c r="B67" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C67" s="47">
-        <f>C4</f>
-        <v>0</v>
-      </c>
-      <c r="D67" s="48"/>
-      <c r="E67" s="47">
-        <f>E4</f>
-        <v>0</v>
-      </c>
-      <c r="F67" s="48"/>
-      <c r="G67" s="47">
-        <f>G4</f>
-        <v>0</v>
-      </c>
-      <c r="H67" s="48"/>
-      <c r="I67" s="47">
-        <f>I4</f>
-        <v>0</v>
-      </c>
-      <c r="J67" s="48"/>
-      <c r="K67" s="47">
-        <f>K4</f>
-        <v>0</v>
-      </c>
-      <c r="L67" s="48"/>
-      <c r="M67" s="47">
-        <f>M4</f>
-        <v>0</v>
-      </c>
-      <c r="N67" s="48"/>
-      <c r="O67" s="47">
-        <f>O4</f>
-        <v>0</v>
-      </c>
-      <c r="P67" s="48"/>
+      <c r="C67" s="32"/>
+      <c r="D67" s="33"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="32"/>
+      <c r="H67" s="33"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="33"/>
+      <c r="K67" s="32"/>
+      <c r="L67" s="33"/>
+      <c r="M67" s="32"/>
+      <c r="N67" s="33"/>
+      <c r="O67" s="32"/>
+      <c r="P67" s="33"/>
       <c r="Q67" s="3"/>
     </row>
     <row r="68" spans="1:17" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A68" s="3"/>
-      <c r="B68" s="66"/>
+      <c r="B68" s="38"/>
       <c r="C68" s="18" t="s">
         <v>32</v>
       </c>
@@ -2869,20 +2827,20 @@
       <c r="B69" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="C69" s="46"/>
-      <c r="D69" s="49"/>
-      <c r="E69" s="46"/>
-      <c r="F69" s="49"/>
-      <c r="G69" s="46"/>
-      <c r="H69" s="49"/>
-      <c r="I69" s="46"/>
-      <c r="J69" s="49"/>
-      <c r="K69" s="46"/>
-      <c r="L69" s="49"/>
-      <c r="M69" s="46"/>
-      <c r="N69" s="49"/>
-      <c r="O69" s="46"/>
-      <c r="P69" s="49"/>
+      <c r="C69" s="34"/>
+      <c r="D69" s="43"/>
+      <c r="E69" s="34"/>
+      <c r="F69" s="43"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="43"/>
+      <c r="I69" s="34"/>
+      <c r="J69" s="43"/>
+      <c r="K69" s="34"/>
+      <c r="L69" s="43"/>
+      <c r="M69" s="34"/>
+      <c r="N69" s="43"/>
+      <c r="O69" s="34"/>
+      <c r="P69" s="43"/>
       <c r="Q69" s="3"/>
     </row>
     <row r="70" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2890,19 +2848,19 @@
       <c r="B70" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C70" s="42"/>
+      <c r="C70" s="35"/>
       <c r="D70" s="44"/>
-      <c r="E70" s="42"/>
+      <c r="E70" s="35"/>
       <c r="F70" s="44"/>
-      <c r="G70" s="42"/>
+      <c r="G70" s="35"/>
       <c r="H70" s="44"/>
-      <c r="I70" s="42"/>
+      <c r="I70" s="35"/>
       <c r="J70" s="44"/>
-      <c r="K70" s="42"/>
+      <c r="K70" s="35"/>
       <c r="L70" s="44"/>
-      <c r="M70" s="42"/>
+      <c r="M70" s="35"/>
       <c r="N70" s="44"/>
-      <c r="O70" s="42"/>
+      <c r="O70" s="35"/>
       <c r="P70" s="44"/>
       <c r="Q70" s="3"/>
     </row>
@@ -2911,19 +2869,19 @@
       <c r="B71" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="C71" s="37"/>
+      <c r="C71" s="41"/>
       <c r="D71" s="39"/>
-      <c r="E71" s="37"/>
+      <c r="E71" s="41"/>
       <c r="F71" s="39"/>
-      <c r="G71" s="37"/>
+      <c r="G71" s="41"/>
       <c r="H71" s="39"/>
-      <c r="I71" s="37"/>
+      <c r="I71" s="41"/>
       <c r="J71" s="39"/>
-      <c r="K71" s="37"/>
+      <c r="K71" s="41"/>
       <c r="L71" s="39"/>
-      <c r="M71" s="37"/>
+      <c r="M71" s="41"/>
       <c r="N71" s="39"/>
-      <c r="O71" s="37"/>
+      <c r="O71" s="41"/>
       <c r="P71" s="39"/>
       <c r="Q71" s="3"/>
     </row>
@@ -2932,19 +2890,19 @@
       <c r="B72" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C72" s="38"/>
+      <c r="C72" s="42"/>
       <c r="D72" s="40"/>
-      <c r="E72" s="38"/>
+      <c r="E72" s="42"/>
       <c r="F72" s="40"/>
-      <c r="G72" s="38"/>
+      <c r="G72" s="42"/>
       <c r="H72" s="40"/>
-      <c r="I72" s="38"/>
+      <c r="I72" s="42"/>
       <c r="J72" s="40"/>
-      <c r="K72" s="38"/>
+      <c r="K72" s="42"/>
       <c r="L72" s="40"/>
-      <c r="M72" s="38"/>
+      <c r="M72" s="42"/>
       <c r="N72" s="40"/>
-      <c r="O72" s="38"/>
+      <c r="O72" s="42"/>
       <c r="P72" s="40"/>
       <c r="Q72" s="3"/>
     </row>
@@ -2953,20 +2911,20 @@
       <c r="B73" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="C73" s="41"/>
-      <c r="D73" s="43"/>
-      <c r="E73" s="41"/>
-      <c r="F73" s="43"/>
-      <c r="G73" s="41"/>
-      <c r="H73" s="43"/>
-      <c r="I73" s="41"/>
-      <c r="J73" s="43"/>
-      <c r="K73" s="41"/>
-      <c r="L73" s="43"/>
-      <c r="M73" s="41"/>
-      <c r="N73" s="43"/>
-      <c r="O73" s="41"/>
-      <c r="P73" s="43"/>
+      <c r="C73" s="45"/>
+      <c r="D73" s="50"/>
+      <c r="E73" s="45"/>
+      <c r="F73" s="50"/>
+      <c r="G73" s="45"/>
+      <c r="H73" s="50"/>
+      <c r="I73" s="45"/>
+      <c r="J73" s="50"/>
+      <c r="K73" s="45"/>
+      <c r="L73" s="50"/>
+      <c r="M73" s="45"/>
+      <c r="N73" s="50"/>
+      <c r="O73" s="45"/>
+      <c r="P73" s="50"/>
       <c r="Q73" s="3"/>
     </row>
     <row r="74" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -2974,19 +2932,19 @@
       <c r="B74" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C74" s="42"/>
+      <c r="C74" s="35"/>
       <c r="D74" s="44"/>
-      <c r="E74" s="42"/>
+      <c r="E74" s="35"/>
       <c r="F74" s="44"/>
-      <c r="G74" s="42"/>
+      <c r="G74" s="35"/>
       <c r="H74" s="44"/>
-      <c r="I74" s="42"/>
+      <c r="I74" s="35"/>
       <c r="J74" s="44"/>
-      <c r="K74" s="42"/>
+      <c r="K74" s="35"/>
       <c r="L74" s="44"/>
-      <c r="M74" s="42"/>
+      <c r="M74" s="35"/>
       <c r="N74" s="44"/>
-      <c r="O74" s="42"/>
+      <c r="O74" s="35"/>
       <c r="P74" s="44"/>
       <c r="Q74" s="3"/>
     </row>
@@ -2995,19 +2953,19 @@
       <c r="B75" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="C75" s="37"/>
+      <c r="C75" s="41"/>
       <c r="D75" s="39"/>
-      <c r="E75" s="37"/>
+      <c r="E75" s="41"/>
       <c r="F75" s="39"/>
-      <c r="G75" s="37"/>
+      <c r="G75" s="41"/>
       <c r="H75" s="39"/>
-      <c r="I75" s="37"/>
+      <c r="I75" s="41"/>
       <c r="J75" s="39"/>
-      <c r="K75" s="37"/>
+      <c r="K75" s="41"/>
       <c r="L75" s="39"/>
-      <c r="M75" s="37"/>
+      <c r="M75" s="41"/>
       <c r="N75" s="39"/>
-      <c r="O75" s="37"/>
+      <c r="O75" s="41"/>
       <c r="P75" s="39"/>
       <c r="Q75" s="3"/>
     </row>
@@ -3016,19 +2974,19 @@
       <c r="B76" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C76" s="38"/>
+      <c r="C76" s="42"/>
       <c r="D76" s="40"/>
-      <c r="E76" s="38"/>
+      <c r="E76" s="42"/>
       <c r="F76" s="40"/>
-      <c r="G76" s="38"/>
+      <c r="G76" s="42"/>
       <c r="H76" s="40"/>
-      <c r="I76" s="38"/>
+      <c r="I76" s="42"/>
       <c r="J76" s="40"/>
-      <c r="K76" s="38"/>
+      <c r="K76" s="42"/>
       <c r="L76" s="40"/>
-      <c r="M76" s="38"/>
+      <c r="M76" s="42"/>
       <c r="N76" s="40"/>
-      <c r="O76" s="38"/>
+      <c r="O76" s="42"/>
       <c r="P76" s="40"/>
       <c r="Q76" s="3"/>
     </row>
@@ -3037,20 +2995,20 @@
       <c r="B77" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C77" s="41"/>
-      <c r="D77" s="43"/>
-      <c r="E77" s="41"/>
-      <c r="F77" s="43"/>
-      <c r="G77" s="41"/>
-      <c r="H77" s="43"/>
-      <c r="I77" s="41"/>
-      <c r="J77" s="43"/>
-      <c r="K77" s="41"/>
-      <c r="L77" s="43"/>
-      <c r="M77" s="41"/>
-      <c r="N77" s="43"/>
-      <c r="O77" s="41"/>
-      <c r="P77" s="43"/>
+      <c r="C77" s="45"/>
+      <c r="D77" s="50"/>
+      <c r="E77" s="45"/>
+      <c r="F77" s="50"/>
+      <c r="G77" s="45"/>
+      <c r="H77" s="50"/>
+      <c r="I77" s="45"/>
+      <c r="J77" s="50"/>
+      <c r="K77" s="45"/>
+      <c r="L77" s="50"/>
+      <c r="M77" s="45"/>
+      <c r="N77" s="50"/>
+      <c r="O77" s="45"/>
+      <c r="P77" s="50"/>
       <c r="Q77" s="3"/>
     </row>
     <row r="78" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
@@ -3058,19 +3016,19 @@
       <c r="B78" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C78" s="42"/>
+      <c r="C78" s="35"/>
       <c r="D78" s="44"/>
-      <c r="E78" s="42"/>
+      <c r="E78" s="35"/>
       <c r="F78" s="44"/>
-      <c r="G78" s="42"/>
+      <c r="G78" s="35"/>
       <c r="H78" s="44"/>
-      <c r="I78" s="42"/>
+      <c r="I78" s="35"/>
       <c r="J78" s="44"/>
-      <c r="K78" s="42"/>
+      <c r="K78" s="35"/>
       <c r="L78" s="44"/>
-      <c r="M78" s="42"/>
+      <c r="M78" s="35"/>
       <c r="N78" s="44"/>
-      <c r="O78" s="42"/>
+      <c r="O78" s="35"/>
       <c r="P78" s="44"/>
       <c r="Q78" s="3"/>
     </row>
@@ -3079,19 +3037,19 @@
       <c r="B79" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C79" s="37"/>
+      <c r="C79" s="41"/>
       <c r="D79" s="39"/>
-      <c r="E79" s="37"/>
+      <c r="E79" s="41"/>
       <c r="F79" s="39"/>
-      <c r="G79" s="37"/>
+      <c r="G79" s="41"/>
       <c r="H79" s="39"/>
-      <c r="I79" s="37"/>
+      <c r="I79" s="41"/>
       <c r="J79" s="39"/>
-      <c r="K79" s="37"/>
+      <c r="K79" s="41"/>
       <c r="L79" s="39"/>
-      <c r="M79" s="37"/>
+      <c r="M79" s="41"/>
       <c r="N79" s="39"/>
-      <c r="O79" s="37"/>
+      <c r="O79" s="41"/>
       <c r="P79" s="39"/>
       <c r="Q79" s="3"/>
     </row>
@@ -3100,172 +3058,172 @@
       <c r="B80" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C80" s="38"/>
+      <c r="C80" s="42"/>
       <c r="D80" s="40"/>
-      <c r="E80" s="38"/>
+      <c r="E80" s="42"/>
       <c r="F80" s="40"/>
-      <c r="G80" s="38"/>
+      <c r="G80" s="42"/>
       <c r="H80" s="40"/>
-      <c r="I80" s="38"/>
+      <c r="I80" s="42"/>
       <c r="J80" s="40"/>
-      <c r="K80" s="38"/>
+      <c r="K80" s="42"/>
       <c r="L80" s="40"/>
-      <c r="M80" s="38"/>
+      <c r="M80" s="42"/>
       <c r="N80" s="40"/>
-      <c r="O80" s="38"/>
+      <c r="O80" s="42"/>
       <c r="P80" s="40"/>
       <c r="Q80" s="3"/>
     </row>
     <row r="81" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3"/>
       <c r="B81" s="14"/>
-      <c r="C81" s="41"/>
-      <c r="D81" s="43"/>
-      <c r="E81" s="41"/>
-      <c r="F81" s="43"/>
-      <c r="G81" s="41"/>
-      <c r="H81" s="43"/>
-      <c r="I81" s="41"/>
-      <c r="J81" s="43"/>
-      <c r="K81" s="41"/>
-      <c r="L81" s="43"/>
-      <c r="M81" s="41"/>
-      <c r="N81" s="43"/>
-      <c r="O81" s="41"/>
-      <c r="P81" s="43"/>
+      <c r="C81" s="45"/>
+      <c r="D81" s="50"/>
+      <c r="E81" s="45"/>
+      <c r="F81" s="50"/>
+      <c r="G81" s="45"/>
+      <c r="H81" s="50"/>
+      <c r="I81" s="45"/>
+      <c r="J81" s="50"/>
+      <c r="K81" s="45"/>
+      <c r="L81" s="50"/>
+      <c r="M81" s="45"/>
+      <c r="N81" s="50"/>
+      <c r="O81" s="45"/>
+      <c r="P81" s="50"/>
       <c r="Q81" s="3"/>
     </row>
     <row r="82" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3"/>
       <c r="B82" s="11"/>
-      <c r="C82" s="42"/>
+      <c r="C82" s="35"/>
       <c r="D82" s="44"/>
-      <c r="E82" s="42"/>
+      <c r="E82" s="35"/>
       <c r="F82" s="44"/>
-      <c r="G82" s="42"/>
+      <c r="G82" s="35"/>
       <c r="H82" s="44"/>
-      <c r="I82" s="42"/>
+      <c r="I82" s="35"/>
       <c r="J82" s="44"/>
-      <c r="K82" s="42"/>
+      <c r="K82" s="35"/>
       <c r="L82" s="44"/>
-      <c r="M82" s="42"/>
+      <c r="M82" s="35"/>
       <c r="N82" s="44"/>
-      <c r="O82" s="42"/>
+      <c r="O82" s="35"/>
       <c r="P82" s="44"/>
       <c r="Q82" s="3"/>
     </row>
     <row r="83" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3"/>
       <c r="B83" s="12"/>
-      <c r="C83" s="37"/>
+      <c r="C83" s="41"/>
       <c r="D83" s="39"/>
-      <c r="E83" s="37"/>
+      <c r="E83" s="41"/>
       <c r="F83" s="39"/>
-      <c r="G83" s="37"/>
+      <c r="G83" s="41"/>
       <c r="H83" s="39"/>
-      <c r="I83" s="37"/>
+      <c r="I83" s="41"/>
       <c r="J83" s="39"/>
-      <c r="K83" s="37"/>
+      <c r="K83" s="41"/>
       <c r="L83" s="39"/>
-      <c r="M83" s="37"/>
+      <c r="M83" s="41"/>
       <c r="N83" s="39"/>
-      <c r="O83" s="37"/>
+      <c r="O83" s="41"/>
       <c r="P83" s="39"/>
       <c r="Q83" s="3"/>
     </row>
     <row r="84" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3"/>
       <c r="B84" s="13"/>
-      <c r="C84" s="38"/>
+      <c r="C84" s="42"/>
       <c r="D84" s="40"/>
-      <c r="E84" s="38"/>
+      <c r="E84" s="42"/>
       <c r="F84" s="40"/>
-      <c r="G84" s="38"/>
+      <c r="G84" s="42"/>
       <c r="H84" s="40"/>
-      <c r="I84" s="38"/>
+      <c r="I84" s="42"/>
       <c r="J84" s="40"/>
-      <c r="K84" s="38"/>
+      <c r="K84" s="42"/>
       <c r="L84" s="40"/>
-      <c r="M84" s="38"/>
+      <c r="M84" s="42"/>
       <c r="N84" s="40"/>
-      <c r="O84" s="38"/>
+      <c r="O84" s="42"/>
       <c r="P84" s="40"/>
       <c r="Q84" s="3"/>
     </row>
     <row r="85" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3"/>
       <c r="B85" s="14"/>
-      <c r="C85" s="41"/>
-      <c r="D85" s="43"/>
-      <c r="E85" s="41"/>
-      <c r="F85" s="43"/>
-      <c r="G85" s="41"/>
-      <c r="H85" s="43"/>
-      <c r="I85" s="41"/>
-      <c r="J85" s="43"/>
-      <c r="K85" s="41"/>
-      <c r="L85" s="43"/>
-      <c r="M85" s="41"/>
-      <c r="N85" s="43"/>
-      <c r="O85" s="41"/>
-      <c r="P85" s="43"/>
+      <c r="C85" s="45"/>
+      <c r="D85" s="50"/>
+      <c r="E85" s="45"/>
+      <c r="F85" s="50"/>
+      <c r="G85" s="45"/>
+      <c r="H85" s="50"/>
+      <c r="I85" s="45"/>
+      <c r="J85" s="50"/>
+      <c r="K85" s="45"/>
+      <c r="L85" s="50"/>
+      <c r="M85" s="45"/>
+      <c r="N85" s="50"/>
+      <c r="O85" s="45"/>
+      <c r="P85" s="50"/>
       <c r="Q85" s="3"/>
     </row>
     <row r="86" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3"/>
       <c r="B86" s="11"/>
-      <c r="C86" s="42"/>
+      <c r="C86" s="35"/>
       <c r="D86" s="44"/>
-      <c r="E86" s="42"/>
+      <c r="E86" s="35"/>
       <c r="F86" s="44"/>
-      <c r="G86" s="42"/>
+      <c r="G86" s="35"/>
       <c r="H86" s="44"/>
-      <c r="I86" s="42"/>
+      <c r="I86" s="35"/>
       <c r="J86" s="44"/>
-      <c r="K86" s="42"/>
+      <c r="K86" s="35"/>
       <c r="L86" s="44"/>
-      <c r="M86" s="42"/>
+      <c r="M86" s="35"/>
       <c r="N86" s="44"/>
-      <c r="O86" s="42"/>
+      <c r="O86" s="35"/>
       <c r="P86" s="44"/>
       <c r="Q86" s="3"/>
     </row>
     <row r="87" spans="1:17" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3"/>
       <c r="B87" s="12"/>
-      <c r="C87" s="37"/>
+      <c r="C87" s="41"/>
       <c r="D87" s="39"/>
-      <c r="E87" s="37"/>
+      <c r="E87" s="41"/>
       <c r="F87" s="39"/>
-      <c r="G87" s="37"/>
+      <c r="G87" s="41"/>
       <c r="H87" s="39"/>
-      <c r="I87" s="37"/>
+      <c r="I87" s="41"/>
       <c r="J87" s="39"/>
-      <c r="K87" s="37"/>
+      <c r="K87" s="41"/>
       <c r="L87" s="39"/>
-      <c r="M87" s="37"/>
+      <c r="M87" s="41"/>
       <c r="N87" s="39"/>
-      <c r="O87" s="37"/>
+      <c r="O87" s="41"/>
       <c r="P87" s="39"/>
       <c r="Q87" s="3"/>
     </row>
     <row r="88" spans="1:17" ht="34.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A88" s="3"/>
       <c r="B88" s="13"/>
-      <c r="C88" s="45"/>
-      <c r="D88" s="57"/>
-      <c r="E88" s="45"/>
-      <c r="F88" s="57"/>
-      <c r="G88" s="45"/>
-      <c r="H88" s="57"/>
-      <c r="I88" s="45"/>
-      <c r="J88" s="57"/>
-      <c r="K88" s="45"/>
-      <c r="L88" s="57"/>
-      <c r="M88" s="45"/>
-      <c r="N88" s="57"/>
-      <c r="O88" s="45"/>
-      <c r="P88" s="57"/>
+      <c r="C88" s="55"/>
+      <c r="D88" s="56"/>
+      <c r="E88" s="55"/>
+      <c r="F88" s="56"/>
+      <c r="G88" s="55"/>
+      <c r="H88" s="56"/>
+      <c r="I88" s="55"/>
+      <c r="J88" s="56"/>
+      <c r="K88" s="55"/>
+      <c r="L88" s="56"/>
+      <c r="M88" s="55"/>
+      <c r="N88" s="56"/>
+      <c r="O88" s="55"/>
+      <c r="P88" s="56"/>
       <c r="Q88" s="3"/>
     </row>
     <row r="89" spans="1:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.35">
@@ -3289,6 +3247,434 @@
     </row>
   </sheetData>
   <mergeCells count="452">
+    <mergeCell ref="B2:N3"/>
+    <mergeCell ref="M79:M80"/>
+    <mergeCell ref="N79:N80"/>
+    <mergeCell ref="M81:M82"/>
+    <mergeCell ref="N81:N82"/>
+    <mergeCell ref="M83:M84"/>
+    <mergeCell ref="N83:N84"/>
+    <mergeCell ref="M85:M86"/>
+    <mergeCell ref="N85:N86"/>
+    <mergeCell ref="M39:M40"/>
+    <mergeCell ref="N39:N40"/>
+    <mergeCell ref="M41:M42"/>
+    <mergeCell ref="N41:N42"/>
+    <mergeCell ref="M43:M44"/>
+    <mergeCell ref="N43:N44"/>
+    <mergeCell ref="M45:M46"/>
+    <mergeCell ref="N45:N46"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="N24:N25"/>
+    <mergeCell ref="M26:M27"/>
+    <mergeCell ref="N26:N27"/>
+    <mergeCell ref="M28:M29"/>
+    <mergeCell ref="M67:N67"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="B65:N66"/>
+    <mergeCell ref="C57:P57"/>
+    <mergeCell ref="N28:N29"/>
+    <mergeCell ref="M35:N35"/>
+    <mergeCell ref="M37:M38"/>
+    <mergeCell ref="N37:N38"/>
+    <mergeCell ref="B33:N34"/>
+    <mergeCell ref="O73:O74"/>
+    <mergeCell ref="P73:P74"/>
+    <mergeCell ref="O69:O70"/>
+    <mergeCell ref="P69:P70"/>
+    <mergeCell ref="D71:D72"/>
+    <mergeCell ref="E71:E72"/>
+    <mergeCell ref="F71:F72"/>
+    <mergeCell ref="G71:G72"/>
+    <mergeCell ref="H71:H72"/>
+    <mergeCell ref="I71:I72"/>
+    <mergeCell ref="J71:J72"/>
+    <mergeCell ref="C47:P47"/>
+    <mergeCell ref="M14:M15"/>
+    <mergeCell ref="N14:N15"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="M20:M21"/>
+    <mergeCell ref="N20:N21"/>
+    <mergeCell ref="M22:M23"/>
+    <mergeCell ref="N22:N23"/>
+    <mergeCell ref="J26:J27"/>
+    <mergeCell ref="K26:K27"/>
+    <mergeCell ref="L26:L27"/>
+    <mergeCell ref="C26:C27"/>
+    <mergeCell ref="D26:D27"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="F26:F27"/>
+    <mergeCell ref="G26:G27"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="M4:N4"/>
+    <mergeCell ref="M6:M7"/>
+    <mergeCell ref="N6:N7"/>
+    <mergeCell ref="M8:M9"/>
+    <mergeCell ref="N8:N9"/>
+    <mergeCell ref="M10:M11"/>
+    <mergeCell ref="N10:N11"/>
+    <mergeCell ref="M12:M13"/>
+    <mergeCell ref="N12:N13"/>
+    <mergeCell ref="O85:O86"/>
+    <mergeCell ref="P85:P86"/>
+    <mergeCell ref="D87:D88"/>
+    <mergeCell ref="E87:E88"/>
+    <mergeCell ref="F87:F88"/>
+    <mergeCell ref="G87:G88"/>
+    <mergeCell ref="H87:H88"/>
+    <mergeCell ref="I87:I88"/>
+    <mergeCell ref="J87:J88"/>
+    <mergeCell ref="K87:K88"/>
+    <mergeCell ref="L87:L88"/>
+    <mergeCell ref="O87:O88"/>
+    <mergeCell ref="P87:P88"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="E85:E86"/>
+    <mergeCell ref="F85:F86"/>
+    <mergeCell ref="G85:G86"/>
+    <mergeCell ref="H85:H86"/>
+    <mergeCell ref="I85:I86"/>
+    <mergeCell ref="J85:J86"/>
+    <mergeCell ref="K85:K86"/>
+    <mergeCell ref="L85:L86"/>
+    <mergeCell ref="M87:M88"/>
+    <mergeCell ref="N87:N88"/>
+    <mergeCell ref="O81:O82"/>
+    <mergeCell ref="P81:P82"/>
+    <mergeCell ref="D83:D84"/>
+    <mergeCell ref="E83:E84"/>
+    <mergeCell ref="F83:F84"/>
+    <mergeCell ref="G83:G84"/>
+    <mergeCell ref="H83:H84"/>
+    <mergeCell ref="I83:I84"/>
+    <mergeCell ref="J83:J84"/>
+    <mergeCell ref="K83:K84"/>
+    <mergeCell ref="L83:L84"/>
+    <mergeCell ref="O83:O84"/>
+    <mergeCell ref="P83:P84"/>
+    <mergeCell ref="D81:D82"/>
+    <mergeCell ref="E81:E82"/>
+    <mergeCell ref="F81:F82"/>
+    <mergeCell ref="G81:G82"/>
+    <mergeCell ref="H81:H82"/>
+    <mergeCell ref="I81:I82"/>
+    <mergeCell ref="J81:J82"/>
+    <mergeCell ref="K81:K82"/>
+    <mergeCell ref="L81:L82"/>
+    <mergeCell ref="O77:O78"/>
+    <mergeCell ref="P77:P78"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="F79:F80"/>
+    <mergeCell ref="G79:G80"/>
+    <mergeCell ref="H79:H80"/>
+    <mergeCell ref="I79:I80"/>
+    <mergeCell ref="J79:J80"/>
+    <mergeCell ref="K79:K80"/>
+    <mergeCell ref="L79:L80"/>
+    <mergeCell ref="O79:O80"/>
+    <mergeCell ref="P79:P80"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="F77:F78"/>
+    <mergeCell ref="G77:G78"/>
+    <mergeCell ref="H77:H78"/>
+    <mergeCell ref="I77:I78"/>
+    <mergeCell ref="J77:J78"/>
+    <mergeCell ref="K77:K78"/>
+    <mergeCell ref="L77:L78"/>
+    <mergeCell ref="M77:M78"/>
+    <mergeCell ref="N77:N78"/>
+    <mergeCell ref="O75:O76"/>
+    <mergeCell ref="P75:P76"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="F73:F74"/>
+    <mergeCell ref="G73:G74"/>
+    <mergeCell ref="H73:H74"/>
+    <mergeCell ref="I73:I74"/>
+    <mergeCell ref="J73:J74"/>
+    <mergeCell ref="K73:K74"/>
+    <mergeCell ref="L73:L74"/>
+    <mergeCell ref="M75:M76"/>
+    <mergeCell ref="N75:N76"/>
+    <mergeCell ref="D75:D76"/>
+    <mergeCell ref="E75:E76"/>
+    <mergeCell ref="F75:F76"/>
+    <mergeCell ref="G75:G76"/>
+    <mergeCell ref="H75:H76"/>
+    <mergeCell ref="I75:I76"/>
+    <mergeCell ref="J75:J76"/>
+    <mergeCell ref="K75:K76"/>
+    <mergeCell ref="L75:L76"/>
+    <mergeCell ref="M73:M74"/>
+    <mergeCell ref="N73:N74"/>
+    <mergeCell ref="K71:K72"/>
+    <mergeCell ref="L71:L72"/>
+    <mergeCell ref="O71:O72"/>
+    <mergeCell ref="P71:P72"/>
+    <mergeCell ref="D69:D70"/>
+    <mergeCell ref="E69:E70"/>
+    <mergeCell ref="F69:F70"/>
+    <mergeCell ref="G69:G70"/>
+    <mergeCell ref="H69:H70"/>
+    <mergeCell ref="I69:I70"/>
+    <mergeCell ref="J69:J70"/>
+    <mergeCell ref="K69:K70"/>
+    <mergeCell ref="L69:L70"/>
+    <mergeCell ref="M69:M70"/>
+    <mergeCell ref="N69:N70"/>
+    <mergeCell ref="M71:M72"/>
+    <mergeCell ref="N71:N72"/>
+    <mergeCell ref="O65:P66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="C67:D67"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="G67:H67"/>
+    <mergeCell ref="I67:J67"/>
+    <mergeCell ref="K67:L67"/>
+    <mergeCell ref="O67:P67"/>
+    <mergeCell ref="O26:O27"/>
+    <mergeCell ref="P26:P27"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="D28:D29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="G28:G29"/>
+    <mergeCell ref="H28:H29"/>
+    <mergeCell ref="I28:I29"/>
+    <mergeCell ref="J28:J29"/>
+    <mergeCell ref="K28:K29"/>
+    <mergeCell ref="L28:L29"/>
+    <mergeCell ref="O28:O29"/>
+    <mergeCell ref="P28:P29"/>
+    <mergeCell ref="H26:H27"/>
+    <mergeCell ref="I26:I27"/>
+    <mergeCell ref="P55:P56"/>
+    <mergeCell ref="H51:H52"/>
+    <mergeCell ref="I51:I52"/>
+    <mergeCell ref="J51:J52"/>
+    <mergeCell ref="K51:K52"/>
+    <mergeCell ref="L51:L52"/>
+    <mergeCell ref="O53:O54"/>
+    <mergeCell ref="P53:P54"/>
+    <mergeCell ref="M51:M52"/>
+    <mergeCell ref="N51:N52"/>
+    <mergeCell ref="M53:M54"/>
+    <mergeCell ref="N55:N56"/>
+    <mergeCell ref="H53:H54"/>
+    <mergeCell ref="I53:I54"/>
+    <mergeCell ref="J53:J54"/>
+    <mergeCell ref="K53:K54"/>
+    <mergeCell ref="L53:L54"/>
+    <mergeCell ref="E55:E56"/>
+    <mergeCell ref="F55:F56"/>
+    <mergeCell ref="G55:G56"/>
+    <mergeCell ref="H55:H56"/>
+    <mergeCell ref="I55:I56"/>
+    <mergeCell ref="J55:J56"/>
+    <mergeCell ref="K55:K56"/>
+    <mergeCell ref="L55:L56"/>
+    <mergeCell ref="O55:O56"/>
+    <mergeCell ref="O43:O44"/>
+    <mergeCell ref="P43:P44"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="D51:D52"/>
+    <mergeCell ref="E51:E52"/>
+    <mergeCell ref="F51:F52"/>
+    <mergeCell ref="G51:G52"/>
+    <mergeCell ref="J45:J46"/>
+    <mergeCell ref="K45:K46"/>
+    <mergeCell ref="L45:L46"/>
+    <mergeCell ref="O45:O46"/>
+    <mergeCell ref="O51:O52"/>
+    <mergeCell ref="P51:P52"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="P45:P46"/>
+    <mergeCell ref="O37:O38"/>
+    <mergeCell ref="P37:P38"/>
+    <mergeCell ref="L41:L42"/>
+    <mergeCell ref="O41:O42"/>
+    <mergeCell ref="P41:P42"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="H37:H38"/>
+    <mergeCell ref="I37:I38"/>
+    <mergeCell ref="J37:J38"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="F41:F42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="H41:H42"/>
+    <mergeCell ref="I41:I42"/>
+    <mergeCell ref="J41:J42"/>
+    <mergeCell ref="K41:K42"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="D53:D54"/>
+    <mergeCell ref="E53:E54"/>
+    <mergeCell ref="F53:F54"/>
+    <mergeCell ref="G53:G54"/>
+    <mergeCell ref="N53:N54"/>
+    <mergeCell ref="M55:M56"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="H43:H44"/>
+    <mergeCell ref="I43:I44"/>
+    <mergeCell ref="J43:J44"/>
+    <mergeCell ref="K43:K44"/>
+    <mergeCell ref="L43:L44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="D43:D44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="F43:F44"/>
+    <mergeCell ref="G43:G44"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="H45:H46"/>
+    <mergeCell ref="I45:I46"/>
+    <mergeCell ref="D55:D56"/>
+    <mergeCell ref="P24:P25"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="F39:F40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="H39:H40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="J39:J40"/>
+    <mergeCell ref="K39:K40"/>
+    <mergeCell ref="L39:L40"/>
+    <mergeCell ref="O39:O40"/>
+    <mergeCell ref="P39:P40"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="D37:D38"/>
+    <mergeCell ref="E37:E38"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="O24:O25"/>
+    <mergeCell ref="C24:C25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="L22:L23"/>
+    <mergeCell ref="O22:O23"/>
+    <mergeCell ref="P22:P23"/>
+    <mergeCell ref="O16:O17"/>
+    <mergeCell ref="P16:P17"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="E20:E21"/>
+    <mergeCell ref="F20:F21"/>
+    <mergeCell ref="G20:G21"/>
+    <mergeCell ref="H20:H21"/>
+    <mergeCell ref="I20:I21"/>
+    <mergeCell ref="J20:J21"/>
+    <mergeCell ref="K20:K21"/>
+    <mergeCell ref="L20:L21"/>
+    <mergeCell ref="O20:O21"/>
+    <mergeCell ref="P20:P21"/>
+    <mergeCell ref="H16:H17"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="J16:J17"/>
+    <mergeCell ref="K16:K17"/>
+    <mergeCell ref="L16:L17"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="C22:C23"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="H22:H23"/>
+    <mergeCell ref="I22:I23"/>
+    <mergeCell ref="J22:J23"/>
+    <mergeCell ref="K22:K23"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="E18:E19"/>
+    <mergeCell ref="F18:F19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="I10:I11"/>
+    <mergeCell ref="J10:J11"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="H18:H19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="J18:J19"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="F16:F17"/>
+    <mergeCell ref="G16:G17"/>
+    <mergeCell ref="K14:K15"/>
+    <mergeCell ref="L14:L15"/>
+    <mergeCell ref="O6:O7"/>
+    <mergeCell ref="P6:P7"/>
+    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="P14:P15"/>
+    <mergeCell ref="C10:C11"/>
+    <mergeCell ref="D10:D11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="I8:I9"/>
+    <mergeCell ref="J8:J9"/>
+    <mergeCell ref="K8:K9"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="O12:O13"/>
+    <mergeCell ref="P12:P13"/>
+    <mergeCell ref="K10:K11"/>
+    <mergeCell ref="L10:L11"/>
+    <mergeCell ref="O10:O11"/>
+    <mergeCell ref="P10:P11"/>
+    <mergeCell ref="F10:F11"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="O33:P34"/>
+    <mergeCell ref="O35:P35"/>
+    <mergeCell ref="O2:P3"/>
+    <mergeCell ref="O4:P4"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="F12:F13"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="I12:I13"/>
+    <mergeCell ref="K35:L35"/>
+    <mergeCell ref="K12:K13"/>
+    <mergeCell ref="L12:L13"/>
+    <mergeCell ref="L6:L7"/>
+    <mergeCell ref="K6:K7"/>
+    <mergeCell ref="P8:P9"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="H14:H15"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="J14:J15"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="I35:J35"/>
     <mergeCell ref="C6:C7"/>
@@ -3313,434 +3699,6 @@
     <mergeCell ref="F24:F25"/>
     <mergeCell ref="G24:G25"/>
     <mergeCell ref="C14:C15"/>
-    <mergeCell ref="O33:P34"/>
-    <mergeCell ref="O35:P35"/>
-    <mergeCell ref="O2:P3"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="E12:E13"/>
-    <mergeCell ref="F12:F13"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="I12:I13"/>
-    <mergeCell ref="K35:L35"/>
-    <mergeCell ref="K12:K13"/>
-    <mergeCell ref="L12:L13"/>
-    <mergeCell ref="L6:L7"/>
-    <mergeCell ref="K6:K7"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="H14:H15"/>
-    <mergeCell ref="I14:I15"/>
-    <mergeCell ref="J14:J15"/>
-    <mergeCell ref="K14:K15"/>
-    <mergeCell ref="L14:L15"/>
-    <mergeCell ref="O6:O7"/>
-    <mergeCell ref="P6:P7"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="P14:P15"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="D10:D11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="I8:I9"/>
-    <mergeCell ref="J8:J9"/>
-    <mergeCell ref="K8:K9"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="O12:O13"/>
-    <mergeCell ref="P12:P13"/>
-    <mergeCell ref="K10:K11"/>
-    <mergeCell ref="L10:L11"/>
-    <mergeCell ref="O10:O11"/>
-    <mergeCell ref="P10:P11"/>
-    <mergeCell ref="F10:F11"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="I10:I11"/>
-    <mergeCell ref="J10:J11"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="H18:H19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="J18:J19"/>
-    <mergeCell ref="E16:E17"/>
-    <mergeCell ref="F16:F17"/>
-    <mergeCell ref="G16:G17"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="D18:D19"/>
-    <mergeCell ref="E18:E19"/>
-    <mergeCell ref="F18:F19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="I22:I23"/>
-    <mergeCell ref="J22:J23"/>
-    <mergeCell ref="K22:K23"/>
-    <mergeCell ref="L22:L23"/>
-    <mergeCell ref="O22:O23"/>
-    <mergeCell ref="P22:P23"/>
-    <mergeCell ref="O16:O17"/>
-    <mergeCell ref="P16:P17"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D20:D21"/>
-    <mergeCell ref="E20:E21"/>
-    <mergeCell ref="F20:F21"/>
-    <mergeCell ref="G20:G21"/>
-    <mergeCell ref="H20:H21"/>
-    <mergeCell ref="I20:I21"/>
-    <mergeCell ref="J20:J21"/>
-    <mergeCell ref="K20:K21"/>
-    <mergeCell ref="L20:L21"/>
-    <mergeCell ref="O20:O21"/>
-    <mergeCell ref="P20:P21"/>
-    <mergeCell ref="H16:H17"/>
-    <mergeCell ref="I16:I17"/>
-    <mergeCell ref="J16:J17"/>
-    <mergeCell ref="K16:K17"/>
-    <mergeCell ref="L16:L17"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="D16:D17"/>
-    <mergeCell ref="P24:P25"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="D39:D40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="F39:F40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="H39:H40"/>
-    <mergeCell ref="I39:I40"/>
-    <mergeCell ref="J39:J40"/>
-    <mergeCell ref="K39:K40"/>
-    <mergeCell ref="L39:L40"/>
-    <mergeCell ref="O39:O40"/>
-    <mergeCell ref="P39:P40"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="D37:D38"/>
-    <mergeCell ref="E37:E38"/>
-    <mergeCell ref="I24:I25"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="O24:O25"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="D53:D54"/>
-    <mergeCell ref="E53:E54"/>
-    <mergeCell ref="F53:F54"/>
-    <mergeCell ref="G53:G54"/>
-    <mergeCell ref="N53:N54"/>
-    <mergeCell ref="M55:M56"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="H43:H44"/>
-    <mergeCell ref="I43:I44"/>
-    <mergeCell ref="J43:J44"/>
-    <mergeCell ref="K43:K44"/>
-    <mergeCell ref="L43:L44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="D43:D44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="F43:F44"/>
-    <mergeCell ref="G43:G44"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="H45:H46"/>
-    <mergeCell ref="I45:I46"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="D41:D42"/>
-    <mergeCell ref="E41:E42"/>
-    <mergeCell ref="F41:F42"/>
-    <mergeCell ref="G41:G42"/>
-    <mergeCell ref="H41:H42"/>
-    <mergeCell ref="I41:I42"/>
-    <mergeCell ref="J41:J42"/>
-    <mergeCell ref="K41:K42"/>
-    <mergeCell ref="O37:O38"/>
-    <mergeCell ref="P37:P38"/>
-    <mergeCell ref="L41:L42"/>
-    <mergeCell ref="O41:O42"/>
-    <mergeCell ref="P41:P42"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="H37:H38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="J37:J38"/>
-    <mergeCell ref="O43:O44"/>
-    <mergeCell ref="P43:P44"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="D51:D52"/>
-    <mergeCell ref="E51:E52"/>
-    <mergeCell ref="F51:F52"/>
-    <mergeCell ref="G51:G52"/>
-    <mergeCell ref="J45:J46"/>
-    <mergeCell ref="K45:K46"/>
-    <mergeCell ref="L45:L46"/>
-    <mergeCell ref="O45:O46"/>
-    <mergeCell ref="O51:O52"/>
-    <mergeCell ref="P51:P52"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="P45:P46"/>
-    <mergeCell ref="D55:D56"/>
-    <mergeCell ref="E55:E56"/>
-    <mergeCell ref="F55:F56"/>
-    <mergeCell ref="G55:G56"/>
-    <mergeCell ref="H55:H56"/>
-    <mergeCell ref="I55:I56"/>
-    <mergeCell ref="J55:J56"/>
-    <mergeCell ref="K55:K56"/>
-    <mergeCell ref="L55:L56"/>
-    <mergeCell ref="O55:O56"/>
-    <mergeCell ref="P55:P56"/>
-    <mergeCell ref="H51:H52"/>
-    <mergeCell ref="I51:I52"/>
-    <mergeCell ref="J51:J52"/>
-    <mergeCell ref="K51:K52"/>
-    <mergeCell ref="L51:L52"/>
-    <mergeCell ref="O53:O54"/>
-    <mergeCell ref="P53:P54"/>
-    <mergeCell ref="M51:M52"/>
-    <mergeCell ref="N51:N52"/>
-    <mergeCell ref="M53:M54"/>
-    <mergeCell ref="N55:N56"/>
-    <mergeCell ref="H53:H54"/>
-    <mergeCell ref="I53:I54"/>
-    <mergeCell ref="J53:J54"/>
-    <mergeCell ref="K53:K54"/>
-    <mergeCell ref="L53:L54"/>
-    <mergeCell ref="O65:P66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="C67:D67"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="G67:H67"/>
-    <mergeCell ref="I67:J67"/>
-    <mergeCell ref="K67:L67"/>
-    <mergeCell ref="O67:P67"/>
-    <mergeCell ref="O26:O27"/>
-    <mergeCell ref="P26:P27"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="D28:D29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
-    <mergeCell ref="G28:G29"/>
-    <mergeCell ref="H28:H29"/>
-    <mergeCell ref="I28:I29"/>
-    <mergeCell ref="J28:J29"/>
-    <mergeCell ref="K28:K29"/>
-    <mergeCell ref="L28:L29"/>
-    <mergeCell ref="O28:O29"/>
-    <mergeCell ref="P28:P29"/>
-    <mergeCell ref="H26:H27"/>
-    <mergeCell ref="I26:I27"/>
-    <mergeCell ref="K71:K72"/>
-    <mergeCell ref="L71:L72"/>
-    <mergeCell ref="O71:O72"/>
-    <mergeCell ref="P71:P72"/>
-    <mergeCell ref="D69:D70"/>
-    <mergeCell ref="E69:E70"/>
-    <mergeCell ref="F69:F70"/>
-    <mergeCell ref="G69:G70"/>
-    <mergeCell ref="H69:H70"/>
-    <mergeCell ref="I69:I70"/>
-    <mergeCell ref="J69:J70"/>
-    <mergeCell ref="K69:K70"/>
-    <mergeCell ref="L69:L70"/>
-    <mergeCell ref="O75:O76"/>
-    <mergeCell ref="P75:P76"/>
-    <mergeCell ref="D73:D74"/>
-    <mergeCell ref="E73:E74"/>
-    <mergeCell ref="F73:F74"/>
-    <mergeCell ref="G73:G74"/>
-    <mergeCell ref="H73:H74"/>
-    <mergeCell ref="I73:I74"/>
-    <mergeCell ref="J73:J74"/>
-    <mergeCell ref="K73:K74"/>
-    <mergeCell ref="L73:L74"/>
-    <mergeCell ref="M75:M76"/>
-    <mergeCell ref="N75:N76"/>
-    <mergeCell ref="D75:D76"/>
-    <mergeCell ref="E75:E76"/>
-    <mergeCell ref="F75:F76"/>
-    <mergeCell ref="G75:G76"/>
-    <mergeCell ref="H75:H76"/>
-    <mergeCell ref="I75:I76"/>
-    <mergeCell ref="J75:J76"/>
-    <mergeCell ref="K75:K76"/>
-    <mergeCell ref="L75:L76"/>
-    <mergeCell ref="O77:O78"/>
-    <mergeCell ref="P77:P78"/>
-    <mergeCell ref="D79:D80"/>
-    <mergeCell ref="E79:E80"/>
-    <mergeCell ref="F79:F80"/>
-    <mergeCell ref="G79:G80"/>
-    <mergeCell ref="H79:H80"/>
-    <mergeCell ref="I79:I80"/>
-    <mergeCell ref="J79:J80"/>
-    <mergeCell ref="K79:K80"/>
-    <mergeCell ref="L79:L80"/>
-    <mergeCell ref="O79:O80"/>
-    <mergeCell ref="P79:P80"/>
-    <mergeCell ref="D77:D78"/>
-    <mergeCell ref="E77:E78"/>
-    <mergeCell ref="F77:F78"/>
-    <mergeCell ref="G77:G78"/>
-    <mergeCell ref="H77:H78"/>
-    <mergeCell ref="I77:I78"/>
-    <mergeCell ref="J77:J78"/>
-    <mergeCell ref="K77:K78"/>
-    <mergeCell ref="L77:L78"/>
-    <mergeCell ref="M77:M78"/>
-    <mergeCell ref="N77:N78"/>
-    <mergeCell ref="O81:O82"/>
-    <mergeCell ref="P81:P82"/>
-    <mergeCell ref="D83:D84"/>
-    <mergeCell ref="E83:E84"/>
-    <mergeCell ref="F83:F84"/>
-    <mergeCell ref="G83:G84"/>
-    <mergeCell ref="H83:H84"/>
-    <mergeCell ref="I83:I84"/>
-    <mergeCell ref="J83:J84"/>
-    <mergeCell ref="K83:K84"/>
-    <mergeCell ref="L83:L84"/>
-    <mergeCell ref="O83:O84"/>
-    <mergeCell ref="P83:P84"/>
-    <mergeCell ref="D81:D82"/>
-    <mergeCell ref="E81:E82"/>
-    <mergeCell ref="F81:F82"/>
-    <mergeCell ref="G81:G82"/>
-    <mergeCell ref="H81:H82"/>
-    <mergeCell ref="I81:I82"/>
-    <mergeCell ref="J81:J82"/>
-    <mergeCell ref="K81:K82"/>
-    <mergeCell ref="L81:L82"/>
-    <mergeCell ref="O85:O86"/>
-    <mergeCell ref="P85:P86"/>
-    <mergeCell ref="D87:D88"/>
-    <mergeCell ref="E87:E88"/>
-    <mergeCell ref="F87:F88"/>
-    <mergeCell ref="G87:G88"/>
-    <mergeCell ref="H87:H88"/>
-    <mergeCell ref="I87:I88"/>
-    <mergeCell ref="J87:J88"/>
-    <mergeCell ref="K87:K88"/>
-    <mergeCell ref="L87:L88"/>
-    <mergeCell ref="O87:O88"/>
-    <mergeCell ref="P87:P88"/>
-    <mergeCell ref="D85:D86"/>
-    <mergeCell ref="E85:E86"/>
-    <mergeCell ref="F85:F86"/>
-    <mergeCell ref="G85:G86"/>
-    <mergeCell ref="H85:H86"/>
-    <mergeCell ref="I85:I86"/>
-    <mergeCell ref="J85:J86"/>
-    <mergeCell ref="K85:K86"/>
-    <mergeCell ref="L85:L86"/>
-    <mergeCell ref="M87:M88"/>
-    <mergeCell ref="N87:N88"/>
-    <mergeCell ref="M4:N4"/>
-    <mergeCell ref="M6:M7"/>
-    <mergeCell ref="N6:N7"/>
-    <mergeCell ref="M8:M9"/>
-    <mergeCell ref="N8:N9"/>
-    <mergeCell ref="M10:M11"/>
-    <mergeCell ref="N10:N11"/>
-    <mergeCell ref="M12:M13"/>
-    <mergeCell ref="N12:N13"/>
-    <mergeCell ref="J26:J27"/>
-    <mergeCell ref="K26:K27"/>
-    <mergeCell ref="L26:L27"/>
-    <mergeCell ref="C26:C27"/>
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="F26:F27"/>
-    <mergeCell ref="G26:G27"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="M14:M15"/>
-    <mergeCell ref="N14:N15"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="M20:M21"/>
-    <mergeCell ref="N20:N21"/>
-    <mergeCell ref="M22:M23"/>
-    <mergeCell ref="N22:N23"/>
-    <mergeCell ref="M69:M70"/>
-    <mergeCell ref="N69:N70"/>
-    <mergeCell ref="M71:M72"/>
-    <mergeCell ref="N71:N72"/>
-    <mergeCell ref="M73:M74"/>
-    <mergeCell ref="N73:N74"/>
-    <mergeCell ref="B65:N66"/>
-    <mergeCell ref="C57:P57"/>
-    <mergeCell ref="N28:N29"/>
-    <mergeCell ref="M35:N35"/>
-    <mergeCell ref="M37:M38"/>
-    <mergeCell ref="N37:N38"/>
-    <mergeCell ref="B33:N34"/>
-    <mergeCell ref="O73:O74"/>
-    <mergeCell ref="P73:P74"/>
-    <mergeCell ref="O69:O70"/>
-    <mergeCell ref="P69:P70"/>
-    <mergeCell ref="D71:D72"/>
-    <mergeCell ref="E71:E72"/>
-    <mergeCell ref="F71:F72"/>
-    <mergeCell ref="G71:G72"/>
-    <mergeCell ref="H71:H72"/>
-    <mergeCell ref="I71:I72"/>
-    <mergeCell ref="J71:J72"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C47:P47"/>
-    <mergeCell ref="B2:N3"/>
-    <mergeCell ref="M79:M80"/>
-    <mergeCell ref="N79:N80"/>
-    <mergeCell ref="M81:M82"/>
-    <mergeCell ref="N81:N82"/>
-    <mergeCell ref="M83:M84"/>
-    <mergeCell ref="N83:N84"/>
-    <mergeCell ref="M85:M86"/>
-    <mergeCell ref="N85:N86"/>
-    <mergeCell ref="M39:M40"/>
-    <mergeCell ref="N39:N40"/>
-    <mergeCell ref="M41:M42"/>
-    <mergeCell ref="N41:N42"/>
-    <mergeCell ref="M43:M44"/>
-    <mergeCell ref="N43:N44"/>
-    <mergeCell ref="M45:M46"/>
-    <mergeCell ref="N45:N46"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="N24:N25"/>
-    <mergeCell ref="M26:M27"/>
-    <mergeCell ref="N26:N27"/>
-    <mergeCell ref="M28:M29"/>
-    <mergeCell ref="M67:N67"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="C1:P46 C47 C48:P56 C57 C58:P1048576">

</xml_diff>